<commit_message>
update cargo.xlsx, update products.xlsx
</commit_message>
<xml_diff>
--- a/Excel/cargo.xlsx
+++ b/Excel/cargo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hugo/Desktop/school-uni-bd6/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C97EE86-8B02-5847-B3C7-6FEC86A7B1A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A88F4EB7-7447-BA4C-B64F-5ADF29573F07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16800" yWindow="500" windowWidth="16800" windowHeight="19100" xr2:uid="{893B05A0-E8CD-47E6-8CBB-CA4954A9E3D0}"/>
   </bookViews>
@@ -398,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F958FDC-8D41-4988-847D-F64B42B1A651}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="139" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -431,7 +431,7 @@
         <v>12</v>
       </c>
       <c r="D2">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -445,7 +445,7 @@
         <v>3</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -459,7 +459,7 @@
         <v>7</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -473,7 +473,7 @@
         <v>26</v>
       </c>
       <c r="D5">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -487,7 +487,7 @@
         <v>7</v>
       </c>
       <c r="D6">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -501,7 +501,7 @@
         <v>6</v>
       </c>
       <c r="D7">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -515,7 +515,7 @@
         <v>24</v>
       </c>
       <c r="D8">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -529,7 +529,7 @@
         <v>19</v>
       </c>
       <c r="D9">
-        <v>21</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -543,7 +543,7 @@
         <v>25</v>
       </c>
       <c r="D10">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -557,7 +557,7 @@
         <v>21</v>
       </c>
       <c r="D11">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -571,7 +571,7 @@
         <v>20</v>
       </c>
       <c r="D12">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -585,7 +585,7 @@
         <v>14</v>
       </c>
       <c r="D13">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -599,7 +599,7 @@
         <v>15</v>
       </c>
       <c r="D14">
-        <v>8</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -607,13 +607,13 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15">
         <v>17</v>
       </c>
       <c r="D15">
-        <v>14</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -627,7 +627,7 @@
         <v>5</v>
       </c>
       <c r="D16">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -641,7 +641,7 @@
         <v>6</v>
       </c>
       <c r="D17">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -655,7 +655,7 @@
         <v>18</v>
       </c>
       <c r="D18">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -663,27 +663,13 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C19">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D19">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <v>4</v>
-      </c>
-      <c r="C20">
-        <v>9</v>
-      </c>
-      <c r="D20">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>